<commit_message>
updated status state definitions
</commit_message>
<xml_diff>
--- a/status_state_definitions.xlsx
+++ b/status_state_definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessel\Documents\GitHub\shs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D06DF19-4078-493B-BD5A-C136CB099444}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAF6C71-86E7-410C-BDA7-4E43C51B5C0F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E28EF7E3-213E-4428-A903-7CE38925DA7D}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$43</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="98">
   <si>
     <t>2019-06-11 12:30:11pm PDT</t>
   </si>
@@ -319,6 +319,21 @@
   </si>
   <si>
     <t>alarm_panel_pold LEGACY</t>
+  </si>
+  <si>
+    <t>50%
+Battery Status</t>
+  </si>
+  <si>
+    <t>{"id":"",
+"key":"",
+"trip_time":"",
+"cur_val":"01",
+"trip_val":"",
+"status_state":10252}</t>
+  </si>
+  <si>
+    <t>Alarm Push</t>
   </si>
 </sst>
 </file>
@@ -871,25 +886,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1212,38 +1227,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FE0F94-C606-40E0-966B-BF1BCBA8A9DE}">
-  <dimension ref="A1:Q45"/>
+  <dimension ref="A1:R44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M42" sqref="M42"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S41" sqref="S41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="105" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="35.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="8"/>
     <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" style="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="1"/>
+    <col min="9" max="9" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="1"/>
     <col min="11" max="11" width="10.85546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="10.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="30.5703125" style="7" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="10"/>
-    <col min="18" max="18" width="21.5703125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="14" width="12.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="29.5703125" style="7" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="10"/>
+    <col min="19" max="19" width="21.5703125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>66</v>
       </c>
@@ -1284,14 +1300,17 @@
         <v>27</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="P1" s="12"/>
-    </row>
-    <row r="2" spans="1:16" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="Q1" s="12"/>
+    </row>
+    <row r="2" spans="1:17" ht="105" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>29</v>
       </c>
@@ -1329,13 +1348,16 @@
       <c r="M2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="53" t="s">
-        <v>3</v>
-      </c>
-      <c r="O2" s="60"/>
-      <c r="P2" s="6"/>
-    </row>
-    <row r="3" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="6"/>
+    </row>
+    <row r="3" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>29</v>
       </c>
@@ -1373,13 +1395,16 @@
       <c r="M3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O3" s="61"/>
-      <c r="P3" s="6"/>
-    </row>
-    <row r="4" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N3" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="6"/>
+    </row>
+    <row r="4" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>29</v>
       </c>
@@ -1417,13 +1442,16 @@
       <c r="M4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O4" s="61"/>
-      <c r="P4" s="6"/>
-    </row>
-    <row r="5" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N4" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="6"/>
+    </row>
+    <row r="5" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>29</v>
       </c>
@@ -1461,13 +1489,16 @@
       <c r="M5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="6"/>
-    </row>
-    <row r="6" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N5" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" s="61"/>
+      <c r="Q5" s="6"/>
+    </row>
+    <row r="6" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>29</v>
       </c>
@@ -1487,11 +1518,14 @@
       <c r="K6" s="29"/>
       <c r="L6" s="29"/>
       <c r="M6" s="29"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="62"/>
-      <c r="P6" s="7"/>
-    </row>
-    <row r="7" spans="1:16" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N6" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="55"/>
+      <c r="P6" s="62"/>
+      <c r="Q6" s="7"/>
+    </row>
+    <row r="7" spans="1:17" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>29</v>
       </c>
@@ -1527,13 +1561,16 @@
       <c r="M7" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="56" t="s">
-        <v>3</v>
-      </c>
-      <c r="O7" s="63"/>
-      <c r="P7" s="6"/>
-    </row>
-    <row r="8" spans="1:16" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N7" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="O7" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="P7" s="63"/>
+      <c r="Q7" s="6"/>
+    </row>
+    <row r="8" spans="1:17" ht="105" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>30</v>
       </c>
@@ -1571,13 +1608,16 @@
       <c r="M8" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="N8" s="53" t="s">
-        <v>3</v>
-      </c>
-      <c r="O8" s="60"/>
-      <c r="P8" s="6"/>
-    </row>
-    <row r="9" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N8" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="O8" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="6"/>
+    </row>
+    <row r="9" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>30</v>
       </c>
@@ -1615,13 +1655,16 @@
       <c r="M9" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N9" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O9" s="61"/>
-      <c r="P9" s="6"/>
-    </row>
-    <row r="10" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N9" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O9" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" s="61"/>
+      <c r="Q9" s="6"/>
+    </row>
+    <row r="10" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>30</v>
       </c>
@@ -1659,13 +1702,16 @@
       <c r="M10" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N10" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O10" s="61"/>
-      <c r="P10" s="6"/>
-    </row>
-    <row r="11" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N10" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O10" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P10" s="61"/>
+      <c r="Q10" s="6"/>
+    </row>
+    <row r="11" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>30</v>
       </c>
@@ -1703,13 +1749,16 @@
       <c r="M11" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N11" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O11" s="61"/>
-      <c r="P11" s="6"/>
-    </row>
-    <row r="12" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N11" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O11" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P11" s="61"/>
+      <c r="Q11" s="6"/>
+    </row>
+    <row r="12" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>30</v>
       </c>
@@ -1729,11 +1778,14 @@
       <c r="K12" s="29"/>
       <c r="L12" s="29"/>
       <c r="M12" s="29"/>
-      <c r="N12" s="55"/>
-      <c r="O12" s="62"/>
-      <c r="P12" s="7"/>
-    </row>
-    <row r="13" spans="1:16" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N12" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="O12" s="55"/>
+      <c r="P12" s="62"/>
+      <c r="Q12" s="7"/>
+    </row>
+    <row r="13" spans="1:17" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="31" t="s">
         <v>30</v>
       </c>
@@ -1769,13 +1821,16 @@
       <c r="M13" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="N13" s="56" t="s">
-        <v>3</v>
-      </c>
-      <c r="O13" s="63"/>
-      <c r="P13" s="6"/>
-    </row>
-    <row r="14" spans="1:16" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N13" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="O13" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="P13" s="63"/>
+      <c r="Q13" s="6"/>
+    </row>
+    <row r="14" spans="1:17" ht="105" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>36</v>
       </c>
@@ -1813,13 +1868,16 @@
       <c r="M14" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="N14" s="53" t="s">
-        <v>3</v>
-      </c>
-      <c r="O14" s="60"/>
-      <c r="P14" s="6"/>
-    </row>
-    <row r="15" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N14" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="O14" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="P14" s="60"/>
+      <c r="Q14" s="6"/>
+    </row>
+    <row r="15" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>36</v>
       </c>
@@ -1857,13 +1915,16 @@
       <c r="M15" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N15" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O15" s="61"/>
-      <c r="P15" s="6"/>
-    </row>
-    <row r="16" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N15" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O15" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P15" s="61"/>
+      <c r="Q15" s="6"/>
+    </row>
+    <row r="16" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>36</v>
       </c>
@@ -1901,13 +1962,16 @@
       <c r="M16" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N16" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O16" s="61"/>
-      <c r="P16" s="6"/>
-    </row>
-    <row r="17" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N16" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O16" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P16" s="61"/>
+      <c r="Q16" s="6"/>
+    </row>
+    <row r="17" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>36</v>
       </c>
@@ -1945,13 +2009,16 @@
       <c r="M17" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N17" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O17" s="61"/>
-      <c r="P17" s="6"/>
-    </row>
-    <row r="18" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N17" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O17" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P17" s="61"/>
+      <c r="Q17" s="6"/>
+    </row>
+    <row r="18" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>36</v>
       </c>
@@ -1971,11 +2038,14 @@
       <c r="K18" s="29"/>
       <c r="L18" s="29"/>
       <c r="M18" s="29"/>
-      <c r="N18" s="55"/>
-      <c r="O18" s="62"/>
-      <c r="P18" s="7"/>
-    </row>
-    <row r="19" spans="1:16" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N18" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="O18" s="55"/>
+      <c r="P18" s="62"/>
+      <c r="Q18" s="7"/>
+    </row>
+    <row r="19" spans="1:17" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="31" t="s">
         <v>36</v>
       </c>
@@ -2011,13 +2081,16 @@
       <c r="M19" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="N19" s="56" t="s">
-        <v>3</v>
-      </c>
-      <c r="O19" s="63"/>
-      <c r="P19" s="6"/>
-    </row>
-    <row r="20" spans="1:16" ht="74.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N19" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="O19" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="P19" s="63"/>
+      <c r="Q19" s="6"/>
+    </row>
+    <row r="20" spans="1:17" ht="105" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>37</v>
       </c>
@@ -2055,13 +2128,16 @@
       <c r="M20" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="N20" s="53" t="s">
-        <v>3</v>
-      </c>
-      <c r="O20" s="60"/>
-      <c r="P20" s="6"/>
-    </row>
-    <row r="21" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N20" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="O20" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="P20" s="60"/>
+      <c r="Q20" s="6"/>
+    </row>
+    <row r="21" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
         <v>37</v>
       </c>
@@ -2099,13 +2175,16 @@
       <c r="M21" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N21" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O21" s="61"/>
-      <c r="P21" s="6"/>
-    </row>
-    <row r="22" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N21" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O21" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P21" s="61"/>
+      <c r="Q21" s="6"/>
+    </row>
+    <row r="22" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>37</v>
       </c>
@@ -2143,13 +2222,16 @@
       <c r="M22" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N22" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O22" s="61"/>
-      <c r="P22" s="6"/>
-    </row>
-    <row r="23" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N22" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O22" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P22" s="61"/>
+      <c r="Q22" s="6"/>
+    </row>
+    <row r="23" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
         <v>37</v>
       </c>
@@ -2187,13 +2269,16 @@
       <c r="M23" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N23" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O23" s="61"/>
-      <c r="P23" s="6"/>
-    </row>
-    <row r="24" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N23" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O23" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P23" s="61"/>
+      <c r="Q23" s="6"/>
+    </row>
+    <row r="24" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
         <v>37</v>
       </c>
@@ -2231,13 +2316,16 @@
       <c r="M24" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N24" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O24" s="61"/>
-      <c r="P24" s="6"/>
-    </row>
-    <row r="25" spans="1:16" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N24" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O24" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P24" s="61"/>
+      <c r="Q24" s="6"/>
+    </row>
+    <row r="25" spans="1:17" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="31" t="s">
         <v>37</v>
       </c>
@@ -2275,13 +2363,16 @@
       <c r="M25" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="N25" s="56" t="s">
-        <v>3</v>
-      </c>
-      <c r="O25" s="63"/>
-      <c r="P25" s="6"/>
-    </row>
-    <row r="26" spans="1:16" ht="87.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N25" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="O25" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="P25" s="63"/>
+      <c r="Q25" s="6"/>
+    </row>
+    <row r="26" spans="1:17" ht="105" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>43</v>
       </c>
@@ -2319,13 +2410,16 @@
       <c r="M26" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="N26" s="53" t="s">
-        <v>3</v>
-      </c>
-      <c r="O26" s="60"/>
-      <c r="P26" s="6"/>
-    </row>
-    <row r="27" spans="1:16" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N26" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="O26" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="P26" s="60"/>
+      <c r="Q26" s="6"/>
+    </row>
+    <row r="27" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>43</v>
       </c>
@@ -2363,13 +2457,16 @@
       <c r="M27" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N27" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O27" s="61"/>
-      <c r="P27" s="6"/>
-    </row>
-    <row r="28" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N27" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O27" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P27" s="61"/>
+      <c r="Q27" s="6"/>
+    </row>
+    <row r="28" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
         <v>43</v>
       </c>
@@ -2407,13 +2504,16 @@
       <c r="M28" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N28" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O28" s="61"/>
-      <c r="P28" s="6"/>
-    </row>
-    <row r="29" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N28" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O28" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P28" s="61"/>
+      <c r="Q28" s="6"/>
+    </row>
+    <row r="29" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
         <v>43</v>
       </c>
@@ -2451,13 +2551,16 @@
       <c r="M29" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N29" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O29" s="61"/>
-      <c r="P29" s="6"/>
-    </row>
-    <row r="30" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N29" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O29" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P29" s="61"/>
+      <c r="Q29" s="6"/>
+    </row>
+    <row r="30" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
         <v>43</v>
       </c>
@@ -2495,13 +2598,16 @@
       <c r="M30" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N30" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O30" s="61"/>
-      <c r="P30" s="6"/>
-    </row>
-    <row r="31" spans="1:16" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N30" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O30" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P30" s="61"/>
+      <c r="Q30" s="6"/>
+    </row>
+    <row r="31" spans="1:17" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="31" t="s">
         <v>43</v>
       </c>
@@ -2539,13 +2645,16 @@
       <c r="M31" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="N31" s="56" t="s">
-        <v>2</v>
-      </c>
-      <c r="O31" s="63"/>
-      <c r="P31" s="6"/>
-    </row>
-    <row r="32" spans="1:16" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N31" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="O31" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="P31" s="63"/>
+      <c r="Q31" s="6"/>
+    </row>
+    <row r="32" spans="1:17" ht="105" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>59</v>
       </c>
@@ -2583,13 +2692,16 @@
       <c r="M32" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="N32" s="53" t="s">
-        <v>3</v>
-      </c>
-      <c r="O32" s="60"/>
-      <c r="P32" s="6"/>
-    </row>
-    <row r="33" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N32" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="O32" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="P32" s="60"/>
+      <c r="Q32" s="6"/>
+    </row>
+    <row r="33" spans="1:18" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
         <v>59</v>
       </c>
@@ -2627,13 +2739,16 @@
       <c r="M33" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N33" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O33" s="61"/>
-      <c r="P33" s="6"/>
-    </row>
-    <row r="34" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N33" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O33" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P33" s="61"/>
+      <c r="Q33" s="6"/>
+    </row>
+    <row r="34" spans="1:18" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>59</v>
       </c>
@@ -2671,13 +2786,16 @@
       <c r="M34" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N34" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O34" s="61"/>
-      <c r="P34" s="6"/>
-    </row>
-    <row r="35" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N34" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O34" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P34" s="61"/>
+      <c r="Q34" s="6"/>
+    </row>
+    <row r="35" spans="1:18" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>59</v>
       </c>
@@ -2715,13 +2833,16 @@
       <c r="M35" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N35" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O35" s="61"/>
-      <c r="P35" s="6"/>
-    </row>
-    <row r="36" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N35" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O35" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P35" s="61"/>
+      <c r="Q35" s="6"/>
+    </row>
+    <row r="36" spans="1:18" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
         <v>59</v>
       </c>
@@ -2759,13 +2880,16 @@
       <c r="M36" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="N36" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="O36" s="61"/>
-      <c r="P36" s="6"/>
-    </row>
-    <row r="37" spans="1:17" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N36" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="O36" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="P36" s="61"/>
+      <c r="Q36" s="6"/>
+    </row>
+    <row r="37" spans="1:18" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="31" t="s">
         <v>59</v>
       </c>
@@ -2803,13 +2927,16 @@
       <c r="M37" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="N37" s="56" t="s">
-        <v>2</v>
-      </c>
-      <c r="O37" s="63"/>
-      <c r="P37" s="6"/>
-    </row>
-    <row r="38" spans="1:17" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N37" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="O37" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="P37" s="63"/>
+      <c r="Q37" s="6"/>
+    </row>
+    <row r="38" spans="1:18" ht="105" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A38" s="38" t="s">
         <v>82</v>
       </c>
@@ -2847,13 +2974,16 @@
       <c r="M38" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="N38" s="57" t="s">
+      <c r="N38" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="O38" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="O38" s="64"/>
-      <c r="P38" s="6"/>
-    </row>
-    <row r="39" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P38" s="64"/>
+      <c r="Q38" s="6"/>
+    </row>
+    <row r="39" spans="1:18" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="43" t="s">
         <v>82</v>
       </c>
@@ -2889,18 +3019,21 @@
       <c r="M39" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="N39" s="58" t="s">
+      <c r="N39" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="O39" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="O39" s="65"/>
-      <c r="P39" s="6"/>
-    </row>
-    <row r="40" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P39" s="65"/>
+      <c r="Q39" s="6"/>
+    </row>
+    <row r="40" spans="1:18" s="15" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="43" t="s">
         <v>82</v>
       </c>
       <c r="B40" s="44" t="s">
-        <v>8</v>
+        <v>92</v>
       </c>
       <c r="C40" s="25"/>
       <c r="D40" s="45"/>
@@ -2913,44 +3046,50 @@
       <c r="G40" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="H40" s="47">
-        <v>0</v>
+      <c r="H40" s="47" t="s">
+        <v>85</v>
       </c>
       <c r="I40" s="47" t="s">
         <v>83</v>
       </c>
       <c r="J40" s="45" t="s">
-        <v>84</v>
+        <v>3</v>
       </c>
       <c r="K40" s="45" t="s">
-        <v>84</v>
+        <v>3</v>
       </c>
       <c r="L40" s="45" t="s">
         <v>84</v>
       </c>
       <c r="M40" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="N40" s="58" t="s">
-        <v>84</v>
-      </c>
-      <c r="O40" s="65"/>
-      <c r="P40" s="6"/>
-    </row>
-    <row r="41" spans="1:17" s="15" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="N40" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="O40" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="P40" s="65" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q40" s="13"/>
+      <c r="R40" s="14"/>
+    </row>
+    <row r="41" spans="1:18" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="43" t="s">
         <v>82</v>
       </c>
       <c r="B41" s="44" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C41" s="25"/>
       <c r="D41" s="45"/>
       <c r="E41" s="45" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="F41" s="46">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G41" s="45" t="s">
         <v>2</v>
@@ -2958,8 +3097,8 @@
       <c r="H41" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="I41" s="47">
-        <v>1</v>
+      <c r="I41" s="47" t="s">
+        <v>95</v>
       </c>
       <c r="J41" s="45" t="s">
         <v>3</v>
@@ -2973,42 +3112,42 @@
       <c r="M41" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="N41" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="O41" s="65"/>
-      <c r="P41" s="13"/>
-      <c r="Q41" s="14"/>
-    </row>
-    <row r="42" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N41" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="O41" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="P41" s="65"/>
+      <c r="Q41" s="6"/>
+    </row>
+    <row r="42" spans="1:18" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="43" t="s">
         <v>82</v>
       </c>
       <c r="B42" s="44" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C42" s="25"/>
       <c r="D42" s="45"/>
-      <c r="E42" s="45" t="s">
-        <v>1</v>
-      </c>
+      <c r="E42" s="45"/>
       <c r="F42" s="46">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G42" s="45" t="s">
         <v>2</v>
       </c>
       <c r="H42" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="I42" s="47">
-        <v>1</v>
+        <v>83</v>
+      </c>
+      <c r="I42" s="47" t="s">
+        <v>83</v>
       </c>
       <c r="J42" s="45" t="s">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="K42" s="45" t="s">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="L42" s="45" t="s">
         <v>84</v>
@@ -3016,95 +3155,61 @@
       <c r="M42" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="N42" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="O42" s="65"/>
-      <c r="P42" s="6"/>
-    </row>
-    <row r="43" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="43" t="s">
+      <c r="N42" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="O42" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="P42" s="65"/>
+      <c r="Q42" s="6"/>
+    </row>
+    <row r="43" spans="1:18" ht="105" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="B43" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
-      <c r="F43" s="46">
+      <c r="B43" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="33"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="50"/>
+      <c r="F43" s="51">
         <v>6</v>
       </c>
-      <c r="G43" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="H43" s="47" t="s">
+      <c r="G43" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="H43" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="I43" s="47" t="s">
+      <c r="I43" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="J43" s="45" t="s">
+      <c r="J43" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="K43" s="45" t="s">
+      <c r="K43" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="L43" s="45" t="s">
+      <c r="L43" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="M43" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="N43" s="58" t="s">
+      <c r="M43" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="N43" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="O43" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="O43" s="65"/>
-      <c r="P43" s="6"/>
-    </row>
-    <row r="44" spans="1:17" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="48" t="s">
-        <v>82</v>
-      </c>
-      <c r="B44" s="49" t="s">
-        <v>87</v>
-      </c>
-      <c r="C44" s="33"/>
-      <c r="D44" s="50"/>
-      <c r="E44" s="50"/>
-      <c r="F44" s="51">
-        <v>6</v>
-      </c>
-      <c r="G44" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="H44" s="52" t="s">
-        <v>83</v>
-      </c>
-      <c r="I44" s="52" t="s">
-        <v>83</v>
-      </c>
-      <c r="J44" s="50" t="s">
-        <v>84</v>
-      </c>
-      <c r="K44" s="50" t="s">
-        <v>84</v>
-      </c>
-      <c r="L44" s="50" t="s">
-        <v>84</v>
-      </c>
-      <c r="M44" s="50" t="s">
-        <v>5</v>
-      </c>
-      <c r="N44" s="59" t="s">
-        <v>84</v>
-      </c>
-      <c r="O44" s="66"/>
-      <c r="P44" s="6"/>
-    </row>
-    <row r="45" spans="1:17" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="P43" s="66"/>
+      <c r="Q43" s="6"/>
+    </row>
+    <row r="44" spans="1:18" ht="105" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:N44" xr:uid="{010EBAA5-DC02-473F-AF32-3CE10C145BBF}"/>
+  <autoFilter ref="A1:O43" xr:uid="{010EBAA5-DC02-473F-AF32-3CE10C145BBF}"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -3116,7 +3221,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>